<commit_message>
benerin posisi export delivery dan invoice
</commit_message>
<xml_diff>
--- a/public/template_report/bill_template.xlsx
+++ b/public/template_report/bill_template.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>PT IBARAKI KOGYO HANAN INDONESIA</t>
   </si>
@@ -456,7 +456,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -469,9 +469,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -636,15 +633,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -669,14 +686,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -695,22 +704,13 @@
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
@@ -722,11 +722,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -762,73 +765,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>111920</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>46298</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1043283" cy="449002"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="3145" b="30939"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="111920" y="46298"/>
-          <a:ext cx="1043283" cy="449002"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>29</xdr:row>
@@ -849,7 +785,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -866,6 +802,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>517113</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1"/>
+          <a:ext cx="1428750" cy="517112"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1137,8 +1117,8 @@
   </sheetPr>
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,120 +1132,120 @@
     <col min="8" max="8" width="8.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" style="19" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="18" customWidth="1"/>
     <col min="12" max="12" width="12" style="1" customWidth="1"/>
     <col min="13" max="13" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="10.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K1" s="31"/>
-    </row>
-    <row r="2" spans="1:12" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="K1" s="30"/>
+    </row>
+    <row r="2" spans="1:12" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="79" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="80"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="27"/>
+      <c r="A3" s="83"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="26"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="17" t="s">
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="16" t="s">
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63"/>
-    </row>
-    <row r="6" spans="1:12" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="81" t="s">
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
+      <c r="L5" s="89"/>
+    </row>
+    <row r="6" spans="1:12" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="45" t="s">
+      <c r="B6" s="84"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="86"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="87"/>
-    </row>
-    <row r="7" spans="1:12" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="82" t="s">
+      <c r="J6" s="87"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88"/>
+    </row>
+    <row r="7" spans="1:12" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="44" t="s">
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
-      <c r="L7" s="63"/>
-    </row>
-    <row r="8" spans="1:12" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+      <c r="L7" s="89"/>
+    </row>
+    <row r="8" spans="1:12" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="90" t="s">
         <v>11</v>
       </c>
@@ -1275,35 +1255,35 @@
       <c r="E8" s="90"/>
       <c r="F8" s="90"/>
       <c r="G8" s="90"/>
-      <c r="H8" s="26"/>
-    </row>
-    <row r="9" spans="1:12" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="24" t="s">
+      <c r="H8" s="25"/>
+    </row>
+    <row r="9" spans="1:12" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="24"/>
-    </row>
-    <row r="10" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="14"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="11"/>
-    </row>
-    <row r="11" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="23"/>
+    </row>
+    <row r="10" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="13"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="91" t="s">
         <v>21</v>
       </c>
@@ -1314,40 +1294,40 @@
       <c r="F11" s="91"/>
       <c r="G11" s="91"/>
       <c r="H11" s="91"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="84"/>
-      <c r="L11" s="84"/>
-    </row>
-    <row r="12" spans="1:12" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="94"/>
-      <c r="B12" s="94"/>
-      <c r="C12" s="94"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="85"/>
-      <c r="L12" s="85"/>
-    </row>
-    <row r="13" spans="1:12" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="94"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="94"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="42"/>
-    </row>
-    <row r="14" spans="1:12" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="9"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+    </row>
+    <row r="12" spans="1:12" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="93"/>
+      <c r="B12" s="93"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="70"/>
+    </row>
+    <row r="13" spans="1:12" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="93"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="41"/>
+    </row>
+    <row r="14" spans="1:12" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="92"/>
       <c r="B14" s="92"/>
       <c r="C14" s="92"/>
@@ -1361,197 +1341,208 @@
       <c r="K14" s="92"/>
       <c r="L14" s="92"/>
     </row>
-    <row r="15" spans="1:12" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="12"/>
-      <c r="K15" s="21"/>
-    </row>
-    <row r="16" spans="1:12" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="K16" s="21"/>
-    </row>
-    <row r="17" spans="1:18" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-    </row>
-    <row r="19" spans="1:18" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+    <row r="15" spans="1:12" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="11"/>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="1:18" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="9"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="19" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="89" t="s">
+      <c r="B19" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="89"/>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="71"/>
+      <c r="D19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="89" t="s">
+      <c r="E19" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="7" t="s">
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="71"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="M19" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="N19" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="K19" s="93" t="s">
+      <c r="O19" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="L19" s="93"/>
-    </row>
-    <row r="20" spans="1:18" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="88"/>
-      <c r="L20" s="88"/>
+      <c r="P19" s="95"/>
+    </row>
+    <row r="20" spans="1:18" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="94"/>
+      <c r="L20" s="94"/>
     </row>
     <row r="21" spans="1:18" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H21" s="19"/>
-      <c r="I21" s="71" t="s">
+      <c r="H21" s="18"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="J21" s="71"/>
-      <c r="K21" s="70"/>
-      <c r="L21" s="70"/>
-      <c r="M21" s="5"/>
+      <c r="N21" s="78"/>
+      <c r="O21" s="45"/>
     </row>
     <row r="22" spans="1:18" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I22" s="71" t="s">
+      <c r="K22" s="77"/>
+      <c r="L22" s="77"/>
+      <c r="M22" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="J22" s="71"/>
-      <c r="K22" s="70"/>
-      <c r="L22" s="70"/>
-    </row>
-    <row r="23" spans="1:18" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J23" s="38" t="s">
+      <c r="N22" s="78"/>
+      <c r="O22" s="45"/>
+    </row>
+    <row r="23" spans="1:18" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
+      <c r="N23" s="78"/>
+      <c r="O23" s="63"/>
     </row>
     <row r="24" spans="1:18" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="70"/>
-      <c r="L24" s="70"/>
-    </row>
-    <row r="25" spans="1:18" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
-    </row>
-    <row r="26" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="78"/>
+      <c r="J24" s="78"/>
+      <c r="K24" s="77"/>
+      <c r="L24" s="77"/>
+    </row>
+    <row r="25" spans="1:18" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="60"/>
+    </row>
+    <row r="26" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="74" t="s">
+    <row r="27" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="60"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="59"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
-      <c r="B28" s="76" t="s">
+    <row r="28" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="54"/>
+      <c r="B28" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="77"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="72"/>
-      <c r="K28" s="72"/>
-      <c r="L28" s="72"/>
-      <c r="M28" s="72"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="67"/>
+      <c r="I28" s="79"/>
+      <c r="J28" s="79"/>
+      <c r="K28" s="79"/>
+      <c r="L28" s="79"/>
+      <c r="M28" s="79"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="52"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-    </row>
-    <row r="30" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
-      <c r="B30" s="65" t="s">
+    <row r="29" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="54"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="51"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+    </row>
+    <row r="30" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="54"/>
+      <c r="B30" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="53"/>
-      <c r="I30" s="73"/>
-      <c r="J30" s="73"/>
-      <c r="K30" s="73"/>
-      <c r="L30" s="73"/>
-      <c r="M30" s="73"/>
-      <c r="N30" s="73"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="52"/>
+      <c r="I30" s="80"/>
+      <c r="J30" s="80"/>
+      <c r="K30" s="80"/>
+      <c r="L30" s="80"/>
+      <c r="M30" s="80"/>
+      <c r="N30" s="80"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
-      <c r="B31" s="65" t="s">
+    <row r="31" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="54"/>
+      <c r="B31" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="53"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="52"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -1563,18 +1554,18 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="56"/>
-      <c r="B32" s="66" t="s">
+    <row r="32" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="55"/>
+      <c r="B32" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="66"/>
-      <c r="D32" s="67" t="s">
+      <c r="C32" s="73"/>
+      <c r="D32" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="68"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="75"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -1586,14 +1577,14 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="56"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="51"/>
+    <row r="33" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="55"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="50"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -1605,39 +1596,39 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="56"/>
-      <c r="B34" s="66" t="s">
+    <row r="34" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="55"/>
+      <c r="B34" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="66"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="66"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="51"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="50"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-      <c r="N34" s="69"/>
-      <c r="O34" s="69"/>
-      <c r="P34" s="69"/>
-      <c r="Q34" s="69"/>
-      <c r="R34" s="69"/>
-    </row>
-    <row r="35" spans="1:18" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
-      <c r="B35" s="49" t="s">
+      <c r="N34" s="76"/>
+      <c r="O34" s="76"/>
+      <c r="P34" s="76"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="76"/>
+    </row>
+    <row r="35" spans="1:18" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="55"/>
+      <c r="B35" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="49"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="51"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="50"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -1645,51 +1636,51 @@
       <c r="M35" s="1"/>
     </row>
     <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="57"/>
-      <c r="B36" s="66" t="s">
+      <c r="A36" s="56"/>
+      <c r="B36" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="66"/>
-      <c r="D36" s="67" t="s">
+      <c r="C36" s="73"/>
+      <c r="D36" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="64" t="s">
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="K36" s="64"/>
-      <c r="L36" s="64"/>
-      <c r="M36" s="36"/>
+      <c r="K36" s="72"/>
+      <c r="L36" s="72"/>
+      <c r="M36" s="35"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="58"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="54"/>
-      <c r="J37" s="64" t="s">
+      <c r="A37" s="57"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="53"/>
+      <c r="J37" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="K37" s="64"/>
-      <c r="L37" s="64"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="72"/>
     </row>
     <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="E19:G19"/>
+  <mergeCells count="43">
+    <mergeCell ref="O19:P19"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A11:H11"/>
     <mergeCell ref="A14:L14"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="K19:L19"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A12:D12"/>
+    <mergeCell ref="I19:K19"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="A3:H3"/>
@@ -1699,17 +1690,18 @@
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J7:L7"/>
     <mergeCell ref="N34:R34"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="K24:L24"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="I28:M28"/>
     <mergeCell ref="I30:N30"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
     <mergeCell ref="J36:L36"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="J37:L37"/>
@@ -1723,13 +1715,13 @@
     <mergeCell ref="B30:F30"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="E19:G19"/>
   </mergeCells>
   <dataValidations count="26">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Quantity in this column under this heading" sqref="A19:A20"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Amount is automatically calculated in this column under this heading and Subtotal is automatically calculated at the end of the table" sqref="K19:K20"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Description in this column under this heading" sqref="D19 J20 D20:H20 B19:B20"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter 'T' for taxable items in this column under this heading" sqref="I19:J19"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Amount is automatically calculated in this column under this heading and Subtotal is automatically calculated at the end of the table" sqref="O19 K20"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Description in this column under this heading" sqref="D19 J20 D20:H20 B19:B20 H19"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter 'T' for taxable items in this column under this heading" sqref="M19:N19"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Comments or Special Instructions in cell at right" sqref="D17:G17 B17"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Company Name in this cell and slogan in cell below. Quotation title is in cell at right" sqref="A2:H2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Company Slogan in this cell and company address in cells below, from cell B4 through B6" sqref="A3:H3"/>
@@ -1745,12 +1737,12 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Quotation end date in this cell" sqref="K11"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter quotation Date in this cell" sqref="J3:J4 K3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Customer ID in cell at right" sqref="I6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter quotation Date in cell at right" sqref="I4 I3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter quotation Date in cell at right" sqref="I3:I4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Quotation number in cell at right" sqref="I5"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter Date, Quotation Number, and Customer ID in cells G2 through G5" sqref="I2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Prepared by name in cell at right" sqref="J12"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Quotation end date in cell at right" sqref="J11"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Unit Price in this column under this heading" sqref="H19"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Unit Price in this column under this heading" sqref="L19"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Comments or Special Instructions in this cell" sqref="H17:L17"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>